<commit_message>
New model seems to be working.
</commit_message>
<xml_diff>
--- a/EV analysis/tables.xlsx
+++ b/EV analysis/tables.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\USER\Documents\GitHub\electromotive-voltage\EV analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\electromotive-voltage\EV analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04F66BD7-D9EB-406B-B2C6-B5F5790DA13D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8C6AE316-D383-425D-81F5-E8DE4AC5AD54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="noise" sheetId="1" r:id="rId1"/>
     <sheet name="imanes" sheetId="2" r:id="rId2"/>
+    <sheet name="distancias" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Sin rectificar</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Int. campo (G)</t>
   </si>
   <si>
-    <t>Intensidad del campo magnético en Gauss para los imanes pequeño y grande.</t>
-  </si>
-  <si>
     <t>Medición</t>
   </si>
   <si>
@@ -74,13 +71,70 @@
   </si>
   <si>
     <t>Desviación del promedio</t>
+  </si>
+  <si>
+    <t>Distancia (cm$\pm$0.05)</t>
+  </si>
+  <si>
+    <t>$z_1$</t>
+  </si>
+  <si>
+    <t>$l$</t>
+  </si>
+  <si>
+    <t>Valor Promedio</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>$4.02\pm0.02$</t>
+  </si>
+  <si>
+    <t>$5.43\pm0.02$</t>
+  </si>
+  <si>
+    <t>Promedio (cm)</t>
+  </si>
+  <si>
+    <t>Intensidad del campo magnético medida con el Gaussmetro para cada imán.</t>
+  </si>
+  <si>
+    <t>Intensidad del campo magnético determinada por el segundo modelo para cada imán.</t>
+  </si>
+  <si>
+    <t>$3300\pm400$</t>
+  </si>
+  <si>
+    <t>$3400\pm500$</t>
+  </si>
+  <si>
+    <t>$3600\pm200$</t>
+  </si>
+  <si>
+    <t>$3400\pm400$</t>
+  </si>
+  <si>
+    <t>$1000\pm60$</t>
+  </si>
+  <si>
+    <t>$940\pm80$</t>
+  </si>
+  <si>
+    <t>$960\pm60$</t>
+  </si>
+  <si>
+    <t>$970\pm70$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +149,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -147,25 +210,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,14 +558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C62607-3920-4735-9DF4-316C45F221D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -530,50 +608,76 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F3D15B-D202-407D-BDB5-89DE0C9445D1}">
-  <dimension ref="B2:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:11">
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="2:11">
+      <c r="B2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
+      <c r="D4" s="5"/>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="F5" s="7"/>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6">
         <v>1</v>
       </c>
@@ -583,8 +687,17 @@
       <c r="D6">
         <v>2979</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7">
         <v>2</v>
       </c>
@@ -594,8 +707,17 @@
       <c r="D7">
         <v>2992</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8">
         <v>3</v>
       </c>
@@ -605,8 +727,17 @@
       <c r="D8">
         <v>2852</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
       <c r="B9">
         <v>4</v>
       </c>
@@ -616,8 +747,17 @@
       <c r="D9">
         <v>2959</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10">
         <v>5</v>
       </c>
@@ -627,8 +767,17 @@
       <c r="D10">
         <v>2965</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
       <c r="B11">
         <v>6</v>
       </c>
@@ -639,7 +788,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:11">
       <c r="B12">
         <v>7</v>
       </c>
@@ -650,7 +799,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:11">
       <c r="B13">
         <v>8</v>
       </c>
@@ -661,7 +810,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:11">
       <c r="B14">
         <v>9</v>
       </c>
@@ -672,46 +821,46 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="5">
+    <row r="15" spans="2:11">
+      <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>2422</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <v>1856</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <f>AVERAGE(C6:C15)</f>
         <v>3366.4</v>
       </c>
       <c r="D16">
-        <f>AVERAGE(D6:D15)</f>
-        <v>2113.1999999999998</v>
+        <f>AVERAGE(D11:D15)</f>
+        <v>1277</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <f>STDEV(C6:C15)</f>
         <v>710.92290564995756</v>
       </c>
       <c r="D17">
-        <f>STDEV(D6:D15)</f>
-        <v>910.24963608891392</v>
+        <f>STDEV(D11:D15)</f>
+        <v>336.21867883863916</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <f>SQRT(C17^2/10)</f>
@@ -719,27 +868,220 @@
       </c>
       <c r="D18">
         <f>SQRT(D17^2/10)</f>
-        <v>287.84620893803697</v>
+        <v>106.32168170227557</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B2:D3"/>
+    <mergeCell ref="F2:H3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="A2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="17"/>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="10">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C4" s="11">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C5" s="13">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13">
+        <v>3.9</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13">
+        <v>3.9</v>
+      </c>
+      <c r="C7" s="13">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="12">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C10" s="13">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13">
+        <v>4</v>
+      </c>
+      <c r="C11" s="13">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C12" s="13">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="14">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14">
+        <v>5.5</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <f>AVERAGE(B4:B13)</f>
+        <v>4.0200000000000005</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGE(C4:C13)</f>
+        <v>5.4299999999999988</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <f>_xlfn.STDEV.P(B4:B13)/SQRT(10)</f>
+        <v>2.3664319132398425E-2</v>
+      </c>
+      <c r="C18">
+        <f>_xlfn.STDEV.P(C4:C13)/SQRT(10)</f>
+        <v>2.0248456731316571E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>